<commit_message>
Added documents. All that is missing is raff's trace matrix
</commit_message>
<xml_diff>
--- a/Documentation/Trace Matrices/Dayton - Trace Matrix.xlsx
+++ b/Documentation/Trace Matrices/Dayton - Trace Matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALGONQUIN\UE\Team TeamTeam\TeamTeam\Documentation\Trace Matrices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Projects\Repos\TeamTeam\Documentation\Trace Matrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AC3761-6341-44F0-908B-67F0AE3BDBFE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0865976E-E8F3-41D7-85A8-EB52271779D6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
   <si>
     <t>Feature/User Story</t>
   </si>
@@ -54,63 +54,18 @@
     <t>Lines</t>
   </si>
   <si>
-    <t>The Hud displays current health.</t>
-  </si>
-  <si>
-    <t>Tilan</t>
-  </si>
-  <si>
     <t>Code</t>
   </si>
   <si>
     <t>../game/src</t>
   </si>
   <si>
-    <t>hud.[cpp,hpp]</t>
-  </si>
-  <si>
-    <t>56-91</t>
-  </si>
-  <si>
-    <t>Font for the HUD.</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
     <t>Art/Design</t>
   </si>
   <si>
-    <t>ZippyFont.fnt</t>
-  </si>
-  <si>
     <t>Entire File</t>
   </si>
   <si>
-    <t>Texture for bullet, AP</t>
-  </si>
-  <si>
-    <t>../game/asset</t>
-  </si>
-  <si>
-    <t>bullet_AP_1.png</t>
-  </si>
-  <si>
-    <t>Audio Packer</t>
-  </si>
-  <si>
-    <t>../Tools/AudioPacker</t>
-  </si>
-  <si>
-    <t>AudioPacker.[cpp,hpp]</t>
-  </si>
-  <si>
-    <t>1-405</t>
-  </si>
-  <si>
-    <t>406-550</t>
-  </si>
-  <si>
     <t>Dayton</t>
   </si>
   <si>
@@ -211,6 +166,12 @@
   </si>
   <si>
     <t>Attempted networking of level layout</t>
+  </si>
+  <si>
+    <t>TDD</t>
+  </si>
+  <si>
+    <t>Documentation</t>
   </si>
 </sst>
 </file>
@@ -704,26 +665,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="2"/>
-    <col min="9" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="39.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="2"/>
+    <col min="9" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -747,367 +708,259 @@
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="G3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="G4" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
-        <v>27</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="3"/>
       <c r="G8" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="F11" s="3"/>
       <c r="G11" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>28</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="9"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="11"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>